<commit_message>
Added further plots in notebook
</commit_message>
<xml_diff>
--- a/test_results/30_32_152.xlsx
+++ b/test_results/30_32_152.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="84">
   <si>
     <t>LIVING_ROOM</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>-30 - MARIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> No</t>
   </si>
   <si>
     <t>+90 - MARIA</t>
@@ -1989,7 +1986,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
@@ -2000,7 +1997,7 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="6" t="s">
@@ -2010,7 +2007,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="4">
         <v>0.0</v>
@@ -2022,11 +2019,11 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -2076,7 +2073,7 @@
         <v>0.0</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -2086,7 +2083,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="9" t="s">
@@ -2130,15 +2127,15 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="4">
         <v>0.0</v>
@@ -2150,13 +2147,13 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="4">
         <v>0.0</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -3230,23 +3227,23 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="4">
         <v>0.0</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="5" t="s">
@@ -3264,7 +3261,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="3"/>
     </row>
@@ -3322,15 +3319,15 @@
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="4">
         <v>0.0</v>
@@ -3338,11 +3335,11 @@
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="4">
         <v>1.0</v>
@@ -3354,11 +3351,11 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="9" t="s">
@@ -3368,7 +3365,7 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="8" t="s">
@@ -3424,37 +3421,37 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="4">
         <v>1.0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -3464,7 +3461,7 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="7" t="s">
@@ -4493,25 +4490,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2">
@@ -4522,19 +4519,19 @@
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3">
@@ -4542,22 +4539,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4">
@@ -4565,19 +4562,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>7</v>
@@ -4588,22 +4585,22 @@
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="6">
@@ -4614,13 +4611,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>7</v>
@@ -4631,16 +4628,16 @@
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" s="12">
         <v>0.6354166666666666</v>
@@ -4654,13 +4651,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="F8" s="12">
         <v>0.6979166666666666</v>
@@ -4671,16 +4668,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="11">
         <v>90.0</v>
@@ -4691,13 +4688,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11">
@@ -4705,13 +4702,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
@@ -4719,13 +4716,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13">
@@ -4736,10 +4733,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>